<commit_message>
Some updates to scenario coverages
</commit_message>
<xml_diff>
--- a/applications/master/data/national/prog_settings.xlsx
+++ b/applications/master/data/national/prog_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/applications/master/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C2401E63-13E9-214F-B6F2-ECB218AC7693}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{46B09C7D-873F-B24A-BCC4-E798031FE097}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26020" yWindow="-20940" windowWidth="19200" windowHeight="21140" firstSheet="1" activeTab="2" xr2:uid="{3C28A406-3B38-3B44-81A1-855DF4E1C8BA}"/>
+    <workbookView xWindow="4120" yWindow="460" windowWidth="19200" windowHeight="15540" firstSheet="2" activeTab="6" xr2:uid="{3C28A406-3B38-3B44-81A1-855DF4E1C8BA}"/>
   </bookViews>
   <sheets>
     <sheet name="IYCF packages" sheetId="7" r:id="rId1"/>
@@ -346,7 +346,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="78">
   <si>
     <t>Coverage</t>
   </si>
@@ -960,8 +960,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
       <sheetData sheetId="3">
         <row r="10">
           <cell r="C10">
@@ -998,9 +998,9 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
       <sheetData sheetId="7">
         <row r="3">
           <cell r="B3">
@@ -1037,7 +1037,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="8"/>
+      <sheetData sheetId="8" refreshError="1"/>
       <sheetData sheetId="9">
         <row r="2">
           <cell r="E2">
@@ -1611,8 +1611,8 @@
   </sheetPr>
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1844,7 +1844,9 @@
       <c r="A37" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="10"/>
+      <c r="B37" s="10" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38" s="38" t="s">
@@ -1856,23 +1858,21 @@
       <c r="A39" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B39" s="10" t="s">
-        <v>5</v>
-      </c>
+      <c r="B39" s="10"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="10" t="s">
-        <v>5</v>
-      </c>
+      <c r="B40" s="10"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A41" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B41" s="10"/>
+      <c r="B41" s="10" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" s="38" t="s">
@@ -1908,13 +1908,17 @@
       <c r="A47" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B47" s="10"/>
+      <c r="B47" s="10" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B48" s="10"/>
+      <c r="B48" s="10" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" s="38" t="s">
@@ -1947,8 +1951,8 @@
   </sheetPr>
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2532,7 +2536,7 @@
         <v>19</v>
       </c>
       <c r="B40" s="15">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C40" s="15">
         <v>0.95</v>
@@ -2606,7 +2610,7 @@
         <v>14</v>
       </c>
       <c r="B45" s="15">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="C45" s="15">
         <v>0.95</v>
@@ -2620,7 +2624,7 @@
         <v>13</v>
       </c>
       <c r="B46" s="15">
-        <v>0.38700000000000001</v>
+        <v>0</v>
       </c>
       <c r="C46" s="15">
         <v>0.95</v>
@@ -2634,7 +2638,7 @@
         <v>12</v>
       </c>
       <c r="B47" s="15">
-        <v>0.69</v>
+        <v>0</v>
       </c>
       <c r="C47" s="15">
         <v>0.95</v>
@@ -2648,7 +2652,7 @@
         <v>11</v>
       </c>
       <c r="B48" s="15">
-        <v>0.84</v>
+        <v>0</v>
       </c>
       <c r="C48" s="15">
         <v>0.95</v>
@@ -2662,7 +2666,7 @@
         <v>10</v>
       </c>
       <c r="B49" s="15">
-        <v>0.14000000000000001</v>
+        <v>0</v>
       </c>
       <c r="C49" s="15">
         <v>0.95</v>
@@ -3351,8 +3355,8 @@
   </sheetPr>
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView zoomScale="94" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="94" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3414,6 +3418,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="40"/>
       <c r="F2" s="41"/>
       <c r="G2" s="41"/>
@@ -4213,9 +4218,7 @@
         <v>0</v>
       </c>
       <c r="C42" s="39"/>
-      <c r="D42" s="40">
-        <v>0.5</v>
-      </c>
+      <c r="D42" s="40"/>
       <c r="F42" s="41"/>
       <c r="G42" s="41"/>
       <c r="H42" s="41"/>
@@ -4234,9 +4237,7 @@
         <v>0</v>
       </c>
       <c r="C43" s="39"/>
-      <c r="D43" s="40">
-        <v>0.5</v>
-      </c>
+      <c r="D43" s="40"/>
       <c r="F43" s="41"/>
       <c r="G43" s="41"/>
       <c r="H43" s="41"/>

</xml_diff>

<commit_message>
Changed some names, easier access to pop projections
</commit_message>
<xml_diff>
--- a/applications/master/data/national/prog_settings.xlsx
+++ b/applications/master/data/national/prog_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/applications/master/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{46B09C7D-873F-B24A-BCC4-E798031FE097}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{38ADDE7F-7D3B-794F-B17E-C2C9F20A0BBB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4120" yWindow="460" windowWidth="19200" windowHeight="15540" firstSheet="2" activeTab="6" xr2:uid="{3C28A406-3B38-3B44-81A1-855DF4E1C8BA}"/>
+    <workbookView xWindow="4120" yWindow="460" windowWidth="19200" windowHeight="15540" activeTab="1" xr2:uid="{3C28A406-3B38-3B44-81A1-855DF4E1C8BA}"/>
   </bookViews>
   <sheets>
     <sheet name="IYCF packages" sheetId="7" r:id="rId1"/>
@@ -346,7 +346,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="78">
   <si>
     <t>Coverage</t>
   </si>
@@ -960,8 +960,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
       <sheetData sheetId="3">
         <row r="10">
           <cell r="C10">
@@ -998,9 +998,9 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
       <sheetData sheetId="7">
         <row r="3">
           <cell r="B3">
@@ -1037,7 +1037,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="8"/>
       <sheetData sheetId="9">
         <row r="2">
           <cell r="E2">
@@ -1611,8 +1611,8 @@
   </sheetPr>
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1844,9 +1844,7 @@
       <c r="A37" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="10" t="s">
-        <v>5</v>
-      </c>
+      <c r="B37" s="10"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38" s="38" t="s">
@@ -1908,17 +1906,13 @@
       <c r="A47" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B47" s="10" t="s">
-        <v>5</v>
-      </c>
+      <c r="B47" s="10"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B48" s="10" t="s">
-        <v>5</v>
-      </c>
+      <c r="B48" s="10"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" s="38" t="s">
@@ -3355,8 +3349,8 @@
   </sheetPr>
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="94" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView zoomScale="94" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>